<commit_message>
Infeasibilities in bigger scenarios
</commit_message>
<xml_diff>
--- a/tests/data/RTS-96.xlsx
+++ b/tests/data/RTS-96.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barberia Juan Luis\Desktop\AnalisisRTS96\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barberia Juan Luis\Desktop\Software\TNEP.py\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ED4D67-2BB5-423B-944E-F979133C0797}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEE2619-22E5-4E9F-BF35-A257F37933C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1080" windowWidth="13185" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parametros" sheetId="1" r:id="rId1"/>
@@ -418,9 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -467,7 +465,7 @@
         <v>500</v>
       </c>
       <c r="H2">
-        <v>38388000</v>
+        <v>38.387999999999998</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -490,7 +488,7 @@
         <v>500</v>
       </c>
       <c r="H3">
-        <v>19194000</v>
+        <v>19.193999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -513,7 +511,7 @@
         <v>500</v>
       </c>
       <c r="H4">
-        <v>32629800</v>
+        <v>32.629800000000003</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -536,7 +534,7 @@
         <v>450</v>
       </c>
       <c r="H5">
-        <v>15355200</v>
+        <v>15.3552</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -559,7 +557,7 @@
         <v>500</v>
       </c>
       <c r="H6">
-        <v>41746950</v>
+        <v>41.746949999999998</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -582,7 +580,7 @@
         <v>500</v>
       </c>
       <c r="H7">
-        <v>23032800</v>
+        <v>23.032800000000002</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -605,7 +603,7 @@
         <v>500</v>
       </c>
       <c r="H8">
-        <v>57582000</v>
+        <v>57.582000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -628,7 +626,7 @@
         <v>500</v>
       </c>
       <c r="H9">
-        <v>34549200</v>
+        <v>34.549199999999999</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -651,7 +649,7 @@
         <v>500</v>
       </c>
       <c r="H10">
-        <v>9597000</v>
+        <v>9.5969999999999995</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -674,7 +672,7 @@
         <v>450</v>
       </c>
       <c r="H11">
-        <v>32629800</v>
+        <v>32.629800000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding ckt ID to branches
</commit_message>
<xml_diff>
--- a/tests/data/RTS-96.xlsx
+++ b/tests/data/RTS-96.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barberia Juan Luis\Desktop\Software\TNEP.py\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEE2619-22E5-4E9F-BF35-A257F37933C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACF88D8-3F09-4869-BE0A-7EB65CC86FF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Bus k</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Costo</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>NL</t>
   </si>
 </sst>
 </file>
@@ -416,13 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,248 +438,281 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>111</v>
       </c>
       <c r="C2">
         <v>115</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.06</v>
       </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2">
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>500</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>38.387999999999998</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>115</v>
       </c>
       <c r="C3">
         <v>119</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>500</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>19.193999999999999</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>115</v>
       </c>
       <c r="C4">
         <v>124</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>500</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>32.629800000000003</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>116</v>
       </c>
       <c r="C5">
         <v>119</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2.3E-2</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>450</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>15.3552</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>116</v>
       </c>
       <c r="C6">
         <v>120</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>6.3E-2</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>500</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>41.746949999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>116</v>
       </c>
       <c r="C7">
         <v>121</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
         <v>2.3E-2</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7">
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>500</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>23.032800000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>213</v>
       </c>
       <c r="C8">
         <v>223</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
         <v>1.2E-2</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8">
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>500</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>57.582000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>215</v>
       </c>
       <c r="C9">
         <v>224</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9">
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>500</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>34.549199999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>217</v>
       </c>
       <c r="C10">
         <v>218</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
         <v>2E-3</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>1.4E-2</v>
       </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10">
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>500</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>9.5969999999999995</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>215</v>
       </c>
       <c r="C11">
         <v>221</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11">
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>450</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>32.629800000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arreglos en la formulacion
</commit_message>
<xml_diff>
--- a/tests/data/RTS-96.xlsx
+++ b/tests/data/RTS-96.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barberia Juan Luis\Desktop\Software\TNEP.py\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barberia Juan Luis\Desktop\TNEP.py\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACF88D8-3F09-4869-BE0A-7EB65CC86FF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7CB378-D330-45B7-84F7-4DC46BD36F6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="13185" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Parametros" sheetId="1" r:id="rId1"/>
+    <sheet name="Candidatas" sheetId="1" r:id="rId1"/>
+    <sheet name="Monitoreadas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>Bus k</t>
   </si>
@@ -425,7 +426,7 @@
   <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I2" sqref="I2:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,4 +720,663 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41AA95A4-31C5-4B46-B1C2-48432C75F1E0}">
+  <dimension ref="B1:E46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>111</v>
+      </c>
+      <c r="C2">
+        <v>113</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>111</v>
+      </c>
+      <c r="C3">
+        <v>114</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>112</v>
+      </c>
+      <c r="C4">
+        <v>113</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>112</v>
+      </c>
+      <c r="C5">
+        <v>123</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>113</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>113</v>
+      </c>
+      <c r="C7">
+        <v>215</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>114</v>
+      </c>
+      <c r="C8">
+        <v>116</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>115</v>
+      </c>
+      <c r="C9">
+        <v>116</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>115</v>
+      </c>
+      <c r="C10">
+        <v>121</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>115</v>
+      </c>
+      <c r="C11">
+        <v>121</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>115</v>
+      </c>
+      <c r="C12">
+        <v>124</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>116</v>
+      </c>
+      <c r="C13">
+        <v>117</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>116</v>
+      </c>
+      <c r="C14">
+        <v>119</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>117</v>
+      </c>
+      <c r="C15">
+        <v>118</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>117</v>
+      </c>
+      <c r="C16">
+        <v>122</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>118</v>
+      </c>
+      <c r="C17">
+        <v>121</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>118</v>
+      </c>
+      <c r="C18">
+        <v>121</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>119</v>
+      </c>
+      <c r="C19">
+        <v>120</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>119</v>
+      </c>
+      <c r="C20">
+        <v>120</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>120</v>
+      </c>
+      <c r="C21">
+        <v>123</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>120</v>
+      </c>
+      <c r="C22">
+        <v>123</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>121</v>
+      </c>
+      <c r="C23">
+        <v>122</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>121</v>
+      </c>
+      <c r="C24">
+        <v>325</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>123</v>
+      </c>
+      <c r="C25">
+        <v>217</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>211</v>
+      </c>
+      <c r="C26">
+        <v>213</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>211</v>
+      </c>
+      <c r="C27">
+        <v>214</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>212</v>
+      </c>
+      <c r="C28">
+        <v>213</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>212</v>
+      </c>
+      <c r="C29">
+        <v>223</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>213</v>
+      </c>
+      <c r="C30">
+        <v>223</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>214</v>
+      </c>
+      <c r="C31">
+        <v>216</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>215</v>
+      </c>
+      <c r="C32">
+        <v>216</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>215</v>
+      </c>
+      <c r="C33">
+        <v>221</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>215</v>
+      </c>
+      <c r="C34">
+        <v>221</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>215</v>
+      </c>
+      <c r="C35">
+        <v>224</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>216</v>
+      </c>
+      <c r="C36">
+        <v>217</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>216</v>
+      </c>
+      <c r="C37">
+        <v>219</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>217</v>
+      </c>
+      <c r="C38">
+        <v>218</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>217</v>
+      </c>
+      <c r="C39">
+        <v>222</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>218</v>
+      </c>
+      <c r="C40">
+        <v>221</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>218</v>
+      </c>
+      <c r="C41">
+        <v>221</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>219</v>
+      </c>
+      <c r="C42">
+        <v>220</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>219</v>
+      </c>
+      <c r="C43">
+        <v>220</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>220</v>
+      </c>
+      <c r="C44">
+        <v>223</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>220</v>
+      </c>
+      <c r="C45">
+        <v>223</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>221</v>
+      </c>
+      <c r="C46">
+        <v>222</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Recorte de carga en parametros
</commit_message>
<xml_diff>
--- a/tests/data/RTS-96.xlsx
+++ b/tests/data/RTS-96.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barberia Juan Luis\Desktop\TNEP.py\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7CB378-D330-45B7-84F7-4DC46BD36F6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756BE3D1-B4AE-4871-BF72-A8522F7B0205}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="13185" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10815" yWindow="480" windowWidth="13185" windowHeight="12420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Candidatas" sheetId="1" r:id="rId1"/>
     <sheet name="Monitoreadas" sheetId="2" r:id="rId2"/>
+    <sheet name="Recorte Carga" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>Bus k</t>
   </si>
@@ -59,6 +60,12 @@
   </si>
   <si>
     <t>NL</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>Recorte Max</t>
   </si>
 </sst>
 </file>
@@ -425,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I11"/>
     </sheetView>
   </sheetViews>
@@ -1379,4 +1386,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5272F9-A4AA-443C-A226-D6E16244A51E}">
+  <dimension ref="C1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>